<commit_message>
start to optimising. blocked by bug
</commit_message>
<xml_diff>
--- a/Progress-notes/data-store.xlsx
+++ b/Progress-notes/data-store.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>timeframe</t>
   </si>
@@ -52,6 +52,15 @@
   </si>
   <si>
     <t>profit factor</t>
+  </si>
+  <si>
+    <t>ac</t>
+  </si>
+  <si>
+    <t>goal</t>
+  </si>
+  <si>
+    <t>best correl-thresh</t>
   </si>
 </sst>
 </file>
@@ -430,61 +439,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="2"/>
-    <col min="5" max="6" width="9.140625" style="1"/>
-    <col min="7" max="7" width="9.140625" style="3"/>
-    <col min="8" max="8" width="9.140625" style="1"/>
-    <col min="9" max="9" width="9.140625" style="3"/>
-    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="5"/>
-    <col min="13" max="13" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="2"/>
+    <col min="6" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="9.140625" style="3"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="9.140625" style="3"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="5"/>
+    <col min="14" max="14" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2">
+        <v>93</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="3">
+        <v>3000</v>
+      </c>
+      <c r="L2">
+        <v>5400</v>
+      </c>
+      <c r="M2" s="5">
+        <v>-700</v>
+      </c>
+      <c r="N2" s="4">
+        <v>0.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first round of optimising len/ac1thresh/correlThresh
</commit_message>
<xml_diff>
--- a/Progress-notes/data-store.xlsx
+++ b/Progress-notes/data-store.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>timeframe</t>
   </si>
@@ -54,13 +54,37 @@
     <t>profit factor</t>
   </si>
   <si>
-    <t>ac</t>
-  </si>
-  <si>
     <t>goal</t>
   </si>
   <si>
     <t>best correl-thresh</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>eur/usd</t>
+  </si>
+  <si>
+    <t>M30</t>
+  </si>
+  <si>
+    <t>ac1</t>
+  </si>
+  <si>
+    <t>processed bars</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>best len</t>
+  </si>
+  <si>
+    <t>best ac1 thresh</t>
+  </si>
+  <si>
+    <t>!no of trades drops dramaticaly with higher ac1, but with better profit factor</t>
   </si>
 </sst>
 </file>
@@ -126,13 +150,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,14 +479,15 @@
     <col min="8" max="8" width="9.140625" style="3"/>
     <col min="9" max="9" width="9.140625" style="1"/>
     <col min="10" max="10" width="9.140625" style="3"/>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="5"/>
-    <col min="14" max="14" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="5"/>
+    <col min="16" max="16" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -491,42 +517,95 @@
         <v>6</v>
       </c>
       <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="Q1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
       </c>
       <c r="D2" s="2">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="G2" s="1">
-        <v>0.4</v>
+        <v>40</v>
+      </c>
+      <c r="H2" s="3">
+        <v>25</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="J2" s="3">
-        <v>3000</v>
-      </c>
-      <c r="L2">
-        <v>5400</v>
-      </c>
-      <c r="M2" s="5">
-        <v>-700</v>
-      </c>
-      <c r="N2" s="4">
-        <v>0.99</v>
+        <v>6000</v>
+      </c>
+      <c r="L2" s="6">
+        <v>42005</v>
+      </c>
+      <c r="M2">
+        <v>10000</v>
+      </c>
+      <c r="N2">
+        <v>60</v>
+      </c>
+      <c r="O2" s="5">
+        <v>1870</v>
+      </c>
+      <c r="P2" s="4">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2">
+        <v>10</v>
+      </c>
+      <c r="L3" s="6"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="1">
+        <v>30</v>
+      </c>
+      <c r="N4">
+        <v>238</v>
+      </c>
+      <c r="O4" s="5">
+        <v>4360</v>
+      </c>
+      <c r="P4" s="4">
+        <v>1.66</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
assessment on HC1&&AC1 added. not beneficial
</commit_message>
<xml_diff>
--- a/Progress-notes/data-store.xlsx
+++ b/Progress-notes/data-store.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>timeframe</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>!no of trades drops dramaticaly with higher ac1, but with better profit factor</t>
+  </si>
+  <si>
+    <t>to 1/4/2016</t>
+  </si>
+  <si>
+    <t>!test on open price similar to all ticks</t>
+  </si>
+  <si>
+    <t>test Hc1ac1</t>
   </si>
 </sst>
 </file>
@@ -464,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,6 +587,9 @@
       <c r="P2" s="4">
         <v>2.6</v>
       </c>
+      <c r="Q2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -587,6 +599,9 @@
         <v>10</v>
       </c>
       <c r="L3" s="6"/>
+      <c r="Q3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -606,6 +621,26 @@
       </c>
       <c r="Q4" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="1">
+        <v>30</v>
+      </c>
+      <c r="G5" s="1">
+        <v>30</v>
+      </c>
+      <c r="N5">
+        <v>90</v>
+      </c>
+      <c r="O5" s="5">
+        <v>750</v>
+      </c>
+      <c r="P5" s="4">
+        <v>1.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
recorded: the result of opt on eur/usd H1 2 years
</commit_message>
<xml_diff>
--- a/Progress-notes/data-store.xlsx
+++ b/Progress-notes/data-store.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>timeframe</t>
   </si>
@@ -94,6 +94,24 @@
   </si>
   <si>
     <t>test Hc1ac1</t>
+  </si>
+  <si>
+    <t>opt on len/correl</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>10+</t>
+  </si>
+  <si>
+    <t>90+</t>
+  </si>
+  <si>
+    <t>thougher conditions, better PF</t>
+  </si>
+  <si>
+    <t>to 1/4/2015</t>
   </si>
 </sst>
 </file>
@@ -473,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,7 +509,7 @@
     <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.140625" style="5"/>
     <col min="16" max="16" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="69.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -641,6 +659,141 @@
       </c>
       <c r="P5" s="4">
         <v>1.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="1">
+        <v>30</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="2">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2">
+        <v>92</v>
+      </c>
+      <c r="G8" s="1">
+        <v>30</v>
+      </c>
+      <c r="H8" s="3">
+        <v>25</v>
+      </c>
+      <c r="J8" s="3">
+        <v>10000</v>
+      </c>
+      <c r="L8" s="6">
+        <v>41275</v>
+      </c>
+      <c r="N8">
+        <v>100</v>
+      </c>
+      <c r="O8" s="5">
+        <v>2100</v>
+      </c>
+      <c r="P8" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="2">
+        <v>18</v>
+      </c>
+      <c r="E9" s="2">
+        <v>86</v>
+      </c>
+      <c r="N9">
+        <v>62</v>
+      </c>
+      <c r="O9" s="5">
+        <v>2000</v>
+      </c>
+      <c r="P9" s="4">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D10" s="2">
+        <v>14</v>
+      </c>
+      <c r="E10" s="2">
+        <v>88</v>
+      </c>
+      <c r="N10">
+        <v>82</v>
+      </c>
+      <c r="O10" s="5">
+        <v>1900</v>
+      </c>
+      <c r="P10" s="4">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D11" s="2">
+        <v>20</v>
+      </c>
+      <c r="E11" s="2">
+        <v>86</v>
+      </c>
+      <c r="N11">
+        <v>50</v>
+      </c>
+      <c r="O11" s="5">
+        <v>1700</v>
+      </c>
+      <c r="P11" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D12" s="2">
+        <v>18</v>
+      </c>
+      <c r="E12" s="2">
+        <v>94</v>
+      </c>
+      <c r="N12">
+        <v>10</v>
+      </c>
+      <c r="O12" s="5">
+        <v>1000</v>
+      </c>
+      <c r="P12" s="4">
+        <v>7.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OPT LOG ON M15
</commit_message>
<xml_diff>
--- a/Progress-notes/data-store.xlsx
+++ b/Progress-notes/data-store.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t>timeframe</t>
   </si>
@@ -72,9 +72,6 @@
     <t>ac1</t>
   </si>
   <si>
-    <t>processed bars</t>
-  </si>
-  <si>
     <t>from</t>
   </si>
   <si>
@@ -111,7 +108,40 @@
     <t>thougher conditions, better PF</t>
   </si>
   <si>
-    <t>to 1/4/2015</t>
+    <t>without opt, taken from H1</t>
+  </si>
+  <si>
+    <t>profitable on M30 based on H1 result</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>lossy on M15 based on H1 result</t>
+  </si>
+  <si>
+    <t>without opt, taken from H2</t>
+  </si>
+  <si>
+    <t>M15</t>
+  </si>
+  <si>
+    <t>opt len and correl</t>
+  </si>
+  <si>
+    <t>opt on M15 seems to be unstable</t>
+  </si>
+  <si>
+    <t>to/processed bars</t>
+  </si>
+  <si>
+    <t>10/2015 - 10000</t>
+  </si>
+  <si>
+    <t>4/2015</t>
   </si>
 </sst>
 </file>
@@ -177,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -185,6 +215,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,10 +575,10 @@
         <v>6</v>
       </c>
       <c r="L1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M1" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="N1" t="s">
         <v>9</v>
@@ -606,24 +637,24 @@
         <v>2.6</v>
       </c>
       <c r="Q2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="2">
         <v>10</v>
       </c>
       <c r="L3" s="6"/>
       <c r="Q3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G4" s="1">
         <v>30</v>
@@ -638,12 +669,12 @@
         <v>1.66</v>
       </c>
       <c r="Q4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" s="1">
         <v>30</v>
@@ -663,25 +694,25 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
       <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="G7" s="1">
         <v>30</v>
       </c>
       <c r="Q7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -689,7 +720,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="2">
         <v>8</v>
@@ -709,6 +740,9 @@
       <c r="L8" s="6">
         <v>41275</v>
       </c>
+      <c r="M8" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="N8">
         <v>100</v>
       </c>
@@ -717,9 +751,6 @@
       </c>
       <c r="P8" s="4">
         <v>1.7</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -727,7 +758,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="2">
         <v>18</v>
@@ -796,8 +827,99 @@
         <v>7.5</v>
       </c>
     </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="2">
+        <v>12</v>
+      </c>
+      <c r="E13" s="2">
+        <v>90</v>
+      </c>
+      <c r="G13" s="1">
+        <v>35</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="2">
+        <v>12</v>
+      </c>
+      <c r="E14" s="2">
+        <v>90</v>
+      </c>
+      <c r="G14" s="1">
+        <v>35</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="2">
+        <v>11</v>
+      </c>
+      <c r="E15" s="2">
+        <v>90</v>
+      </c>
+      <c r="G15" s="1">
+        <v>35</v>
+      </c>
+      <c r="L15" s="6">
+        <v>42005</v>
+      </c>
+      <c r="M15" t="s">
+        <v>40</v>
+      </c>
+      <c r="N15">
+        <v>80</v>
+      </c>
+      <c r="O15" s="5">
+        <v>670</v>
+      </c>
+      <c r="P15" s="4">
+        <v>1.37</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
opted gbp/jpy; eur/usd values didn't work. but opt result worked on another interval
</commit_message>
<xml_diff>
--- a/Progress-notes/data-store.xlsx
+++ b/Progress-notes/data-store.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>timeframe</t>
   </si>
@@ -142,6 +142,18 @@
   </si>
   <si>
     <t>4/2015</t>
+  </si>
+  <si>
+    <t>gbp/jpy</t>
+  </si>
+  <si>
+    <t>opt len and correl1</t>
+  </si>
+  <si>
+    <t>opt len and correl2</t>
+  </si>
+  <si>
+    <t>Re-date</t>
   </si>
 </sst>
 </file>
@@ -207,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -215,6 +227,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -522,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,7 +753,7 @@
       <c r="L8" s="6">
         <v>41275</v>
       </c>
-      <c r="M8" s="7" t="s">
+      <c r="M8" s="8" t="s">
         <v>41</v>
       </c>
       <c r="N8">
@@ -915,6 +928,113 @@
       </c>
       <c r="Q15" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="2">
+        <v>8</v>
+      </c>
+      <c r="E16" s="2">
+        <v>93</v>
+      </c>
+      <c r="L16" s="7">
+        <v>42614</v>
+      </c>
+      <c r="M16" s="7">
+        <v>42887</v>
+      </c>
+      <c r="N16">
+        <v>52</v>
+      </c>
+      <c r="O16" s="5">
+        <v>2600</v>
+      </c>
+      <c r="P16" s="4">
+        <v>1.74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="L17" s="7">
+        <v>41518</v>
+      </c>
+      <c r="M17" s="7">
+        <v>42156</v>
+      </c>
+      <c r="N17">
+        <v>63</v>
+      </c>
+      <c r="O17" s="5">
+        <v>-1000</v>
+      </c>
+      <c r="P17" s="4">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="2">
+        <v>14</v>
+      </c>
+      <c r="E18" s="2">
+        <v>93</v>
+      </c>
+      <c r="G18" s="1">
+        <v>35</v>
+      </c>
+      <c r="L18" s="7">
+        <v>42614</v>
+      </c>
+      <c r="M18" s="7">
+        <v>42887</v>
+      </c>
+      <c r="N18">
+        <v>27</v>
+      </c>
+      <c r="O18" s="5">
+        <v>1200</v>
+      </c>
+      <c r="P18" s="4">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="L19" s="7">
+        <v>41518</v>
+      </c>
+      <c r="M19" s="7">
+        <v>42156</v>
+      </c>
+      <c r="N19">
+        <v>31</v>
+      </c>
+      <c r="O19" s="5">
+        <v>700</v>
+      </c>
+      <c r="P19" s="4">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
recording opt results so far
</commit_message>
<xml_diff>
--- a/Progress-notes/data-store.xlsx
+++ b/Progress-notes/data-store.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
   <si>
     <t>timeframe</t>
   </si>
@@ -123,9 +123,6 @@
     <t>lossy on M15 based on H1 result</t>
   </si>
   <si>
-    <t>without opt, taken from H2</t>
-  </si>
-  <si>
     <t>M15</t>
   </si>
   <si>
@@ -154,16 +151,35 @@
   </si>
   <si>
     <t>Re-date</t>
+  </si>
+  <si>
+    <t>opt on ac1</t>
+  </si>
+  <si>
+    <t>stable opt</t>
+  </si>
+  <si>
+    <t>opt on ac1-Re-date</t>
+  </si>
+  <si>
+    <t>stable opt; But, the opt result is not stable over time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -219,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -229,6 +245,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,7 +552,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
@@ -543,15 +560,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9.140625" style="2"/>
     <col min="6" max="7" width="9.140625" style="1"/>
     <col min="8" max="8" width="9.140625" style="3"/>
     <col min="9" max="9" width="9.140625" style="1"/>
     <col min="10" max="10" width="9.140625" style="3"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="5"/>
+    <col min="14" max="14" width="9.140625" style="5"/>
+    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="69.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -591,13 +608,13 @@
         <v>18</v>
       </c>
       <c r="M1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" t="s">
         <v>9</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="P1" s="4" t="s">
         <v>11</v>
@@ -640,11 +657,11 @@
       <c r="M2">
         <v>10000</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="5">
+        <v>1870</v>
+      </c>
+      <c r="O2">
         <v>60</v>
-      </c>
-      <c r="O2" s="5">
-        <v>1870</v>
       </c>
       <c r="P2" s="4">
         <v>2.6</v>
@@ -672,11 +689,12 @@
       <c r="G4" s="1">
         <v>30</v>
       </c>
-      <c r="N4">
+      <c r="L4" s="6"/>
+      <c r="N4" s="5">
+        <v>4360</v>
+      </c>
+      <c r="O4">
         <v>238</v>
-      </c>
-      <c r="O4" s="5">
-        <v>4360</v>
       </c>
       <c r="P4" s="4">
         <v>1.66</v>
@@ -695,15 +713,19 @@
       <c r="G5" s="1">
         <v>30</v>
       </c>
-      <c r="N5">
+      <c r="L5" s="6"/>
+      <c r="N5" s="5">
+        <v>750</v>
+      </c>
+      <c r="O5">
         <v>90</v>
-      </c>
-      <c r="O5" s="5">
-        <v>750</v>
       </c>
       <c r="P5" s="4">
         <v>1.3</v>
       </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L6" s="6"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -724,6 +746,7 @@
       <c r="G7" s="1">
         <v>30</v>
       </c>
+      <c r="L7" s="6"/>
       <c r="Q7" t="s">
         <v>29</v>
       </c>
@@ -754,13 +777,13 @@
         <v>41275</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="N8">
+        <v>40</v>
+      </c>
+      <c r="N8" s="5">
+        <v>2100</v>
+      </c>
+      <c r="O8">
         <v>100</v>
-      </c>
-      <c r="O8" s="5">
-        <v>2100</v>
       </c>
       <c r="P8" s="4">
         <v>1.7</v>
@@ -779,11 +802,12 @@
       <c r="E9" s="2">
         <v>86</v>
       </c>
-      <c r="N9">
+      <c r="L9" s="6"/>
+      <c r="N9" s="5">
+        <v>2000</v>
+      </c>
+      <c r="O9">
         <v>62</v>
-      </c>
-      <c r="O9" s="5">
-        <v>2000</v>
       </c>
       <c r="P9" s="4">
         <v>2.4</v>
@@ -796,11 +820,12 @@
       <c r="E10" s="2">
         <v>88</v>
       </c>
-      <c r="N10">
+      <c r="L10" s="6"/>
+      <c r="N10" s="5">
+        <v>1900</v>
+      </c>
+      <c r="O10">
         <v>82</v>
-      </c>
-      <c r="O10" s="5">
-        <v>1900</v>
       </c>
       <c r="P10" s="4">
         <v>1.7</v>
@@ -813,11 +838,12 @@
       <c r="E11" s="2">
         <v>86</v>
       </c>
-      <c r="N11">
+      <c r="L11" s="6"/>
+      <c r="N11" s="5">
+        <v>1700</v>
+      </c>
+      <c r="O11">
         <v>50</v>
-      </c>
-      <c r="O11" s="5">
-        <v>1700</v>
       </c>
       <c r="P11" s="4">
         <v>2</v>
@@ -830,11 +856,12 @@
       <c r="E12" s="2">
         <v>94</v>
       </c>
-      <c r="N12">
+      <c r="L12" s="6"/>
+      <c r="N12" s="5">
+        <v>1000</v>
+      </c>
+      <c r="O12">
         <v>10</v>
-      </c>
-      <c r="O12" s="5">
-        <v>1000</v>
       </c>
       <c r="P12" s="4">
         <v>7.5</v>
@@ -859,7 +886,8 @@
       <c r="G13" s="1">
         <v>35</v>
       </c>
-      <c r="O13" s="5" t="s">
+      <c r="L13" s="6"/>
+      <c r="N13" s="5" t="s">
         <v>32</v>
       </c>
       <c r="Q13" t="s">
@@ -868,13 +896,13 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="2">
         <v>12</v>
@@ -885,7 +913,8 @@
       <c r="G14" s="1">
         <v>35</v>
       </c>
-      <c r="O14" s="5" t="s">
+      <c r="L14" s="6"/>
+      <c r="N14" s="5" t="s">
         <v>33</v>
       </c>
       <c r="Q14" t="s">
@@ -894,13 +923,13 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="2">
         <v>11</v>
@@ -915,27 +944,27 @@
         <v>42005</v>
       </c>
       <c r="M15" t="s">
-        <v>40</v>
-      </c>
-      <c r="N15">
+        <v>39</v>
+      </c>
+      <c r="N15" s="5">
+        <v>670</v>
+      </c>
+      <c r="O15">
         <v>80</v>
-      </c>
-      <c r="O15" s="5">
-        <v>670</v>
       </c>
       <c r="P15" s="4">
         <v>1.37</v>
       </c>
       <c r="Q15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
         <v>26</v>
@@ -946,48 +975,48 @@
       <c r="E16" s="2">
         <v>93</v>
       </c>
-      <c r="L16" s="7">
+      <c r="L16" s="6">
         <v>42614</v>
       </c>
       <c r="M16" s="7">
         <v>42887</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="5">
+        <v>2600</v>
+      </c>
+      <c r="O16">
         <v>52</v>
-      </c>
-      <c r="O16" s="5">
-        <v>2600</v>
       </c>
       <c r="P16" s="4">
         <v>1.74</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>45</v>
-      </c>
-      <c r="L17" s="7">
+        <v>44</v>
+      </c>
+      <c r="L17" s="6">
         <v>41518</v>
       </c>
       <c r="M17" s="7">
         <v>42156</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="5">
+        <v>-1000</v>
+      </c>
+      <c r="O17">
         <v>63</v>
-      </c>
-      <c r="O17" s="5">
-        <v>-1000</v>
       </c>
       <c r="P17" s="4">
         <v>0.76</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
@@ -1001,40 +1030,163 @@
       <c r="G18" s="1">
         <v>35</v>
       </c>
-      <c r="L18" s="7">
+      <c r="L18" s="6">
         <v>42614</v>
       </c>
       <c r="M18" s="7">
         <v>42887</v>
       </c>
-      <c r="N18">
+      <c r="N18" s="5">
+        <v>1200</v>
+      </c>
+      <c r="O18">
         <v>27</v>
-      </c>
-      <c r="O18" s="5">
-        <v>1200</v>
       </c>
       <c r="P18" s="4">
         <v>1.7</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>45</v>
-      </c>
-      <c r="L19" s="7">
+        <v>44</v>
+      </c>
+      <c r="L19" s="6">
         <v>41518</v>
       </c>
       <c r="M19" s="7">
         <v>42156</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="5">
+        <v>700</v>
+      </c>
+      <c r="O19">
         <v>31</v>
-      </c>
-      <c r="O19" s="5">
-        <v>700</v>
       </c>
       <c r="P19" s="4">
         <v>1.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="2">
+        <v>12</v>
+      </c>
+      <c r="E20" s="2">
+        <v>90</v>
+      </c>
+      <c r="G20" s="9">
+        <v>40</v>
+      </c>
+      <c r="J20" s="3">
+        <v>6000</v>
+      </c>
+      <c r="L20" s="6">
+        <v>42005</v>
+      </c>
+      <c r="M20" s="6">
+        <v>42736</v>
+      </c>
+      <c r="N20" s="5">
+        <v>650</v>
+      </c>
+      <c r="O20">
+        <v>24</v>
+      </c>
+      <c r="P20" s="4">
+        <v>1.44</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="2">
+        <v>12</v>
+      </c>
+      <c r="E21" s="2">
+        <v>90</v>
+      </c>
+      <c r="G21" s="9">
+        <v>45</v>
+      </c>
+      <c r="J21" s="3">
+        <v>6000</v>
+      </c>
+      <c r="L21" s="6">
+        <v>41640</v>
+      </c>
+      <c r="M21" s="6">
+        <v>42370</v>
+      </c>
+      <c r="N21" s="5">
+        <v>670</v>
+      </c>
+      <c r="O21">
+        <v>12</v>
+      </c>
+      <c r="P21" s="4">
+        <v>3</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="2">
+        <v>12</v>
+      </c>
+      <c r="E22" s="2">
+        <v>90</v>
+      </c>
+      <c r="G22" s="9">
+        <v>30</v>
+      </c>
+      <c r="J22" s="3">
+        <v>6000</v>
+      </c>
+      <c r="L22" s="6">
+        <v>41275</v>
+      </c>
+      <c r="M22" s="6">
+        <v>42005</v>
+      </c>
+      <c r="N22" s="5">
+        <v>1400</v>
+      </c>
+      <c r="O22">
+        <v>128</v>
+      </c>
+      <c r="P22" s="4">
+        <v>1.24</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
optimised for len=10 for live trade; TODO: othre lens and combining them
</commit_message>
<xml_diff>
--- a/Progress-notes/data-store.xlsx
+++ b/Progress-notes/data-store.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
   <si>
     <t>timeframe</t>
   </si>
@@ -163,6 +163,24 @@
   </si>
   <si>
     <t>stable opt; But, the opt result is not stable over time</t>
+  </si>
+  <si>
+    <t>opt on lookback len</t>
+  </si>
+  <si>
+    <t>tp</t>
+  </si>
+  <si>
+    <t>sl</t>
+  </si>
+  <si>
+    <t>keep the live period on 1 year…</t>
+  </si>
+  <si>
+    <t>by adjusting the start day</t>
+  </si>
+  <si>
+    <t>use for live trade</t>
   </si>
 </sst>
 </file>
@@ -552,10 +570,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:S62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,14 +585,14 @@
     <col min="6" max="7" width="9.140625" style="1"/>
     <col min="8" max="8" width="9.140625" style="3"/>
     <col min="9" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="9.140625" style="3"/>
-    <col min="14" max="14" width="9.140625" style="5"/>
-    <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="69.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="9.140625" style="3"/>
+    <col min="16" max="16" width="9.140625" style="5"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="69.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -604,26 +623,32 @@
       <c r="J1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L1" t="s">
+      <c r="K1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -651,59 +676,59 @@
       <c r="J2" s="3">
         <v>6000</v>
       </c>
-      <c r="L2" s="6">
+      <c r="N2" s="6">
         <v>42005</v>
       </c>
-      <c r="M2">
+      <c r="O2">
         <v>10000</v>
       </c>
-      <c r="N2" s="5">
+      <c r="P2" s="5">
         <v>1870</v>
       </c>
-      <c r="O2">
+      <c r="Q2">
         <v>60</v>
       </c>
-      <c r="P2" s="4">
+      <c r="R2" s="4">
         <v>2.6</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
       <c r="D3" s="2">
         <v>10</v>
       </c>
-      <c r="L3" s="6"/>
-      <c r="Q3" t="s">
+      <c r="N3" s="6"/>
+      <c r="S3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="G4" s="1">
         <v>30</v>
       </c>
-      <c r="L4" s="6"/>
-      <c r="N4" s="5">
+      <c r="N4" s="6"/>
+      <c r="P4" s="5">
         <v>4360</v>
       </c>
-      <c r="O4">
+      <c r="Q4">
         <v>238</v>
       </c>
-      <c r="P4" s="4">
+      <c r="R4" s="4">
         <v>1.66</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="S4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -713,21 +738,21 @@
       <c r="G5" s="1">
         <v>30</v>
       </c>
-      <c r="L5" s="6"/>
-      <c r="N5" s="5">
+      <c r="N5" s="6"/>
+      <c r="P5" s="5">
         <v>750</v>
       </c>
-      <c r="O5">
+      <c r="Q5">
         <v>90</v>
       </c>
-      <c r="P5" s="4">
+      <c r="R5" s="4">
         <v>1.3</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="L6" s="6"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N6" s="6"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -746,12 +771,12 @@
       <c r="G7" s="1">
         <v>30</v>
       </c>
-      <c r="L7" s="6"/>
-      <c r="Q7" t="s">
+      <c r="N7" s="6"/>
+      <c r="S7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>15</v>
       </c>
@@ -773,23 +798,23 @@
       <c r="J8" s="3">
         <v>10000</v>
       </c>
-      <c r="L8" s="6">
+      <c r="N8" s="6">
         <v>41275</v>
       </c>
-      <c r="M8" s="8" t="s">
+      <c r="O8" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="N8" s="5">
+      <c r="P8" s="5">
         <v>2100</v>
       </c>
-      <c r="O8">
+      <c r="Q8">
         <v>100</v>
       </c>
-      <c r="P8" s="4">
+      <c r="R8" s="4">
         <v>1.7</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -802,72 +827,72 @@
       <c r="E9" s="2">
         <v>86</v>
       </c>
-      <c r="L9" s="6"/>
-      <c r="N9" s="5">
+      <c r="N9" s="6"/>
+      <c r="P9" s="5">
         <v>2000</v>
       </c>
-      <c r="O9">
+      <c r="Q9">
         <v>62</v>
       </c>
-      <c r="P9" s="4">
+      <c r="R9" s="4">
         <v>2.4</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D10" s="2">
         <v>14</v>
       </c>
       <c r="E10" s="2">
         <v>88</v>
       </c>
-      <c r="L10" s="6"/>
-      <c r="N10" s="5">
+      <c r="N10" s="6"/>
+      <c r="P10" s="5">
         <v>1900</v>
       </c>
-      <c r="O10">
+      <c r="Q10">
         <v>82</v>
       </c>
-      <c r="P10" s="4">
+      <c r="R10" s="4">
         <v>1.7</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D11" s="2">
         <v>20</v>
       </c>
       <c r="E11" s="2">
         <v>86</v>
       </c>
-      <c r="L11" s="6"/>
-      <c r="N11" s="5">
+      <c r="N11" s="6"/>
+      <c r="P11" s="5">
         <v>1700</v>
       </c>
-      <c r="O11">
+      <c r="Q11">
         <v>50</v>
       </c>
-      <c r="P11" s="4">
+      <c r="R11" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D12" s="2">
         <v>18</v>
       </c>
       <c r="E12" s="2">
         <v>94</v>
       </c>
-      <c r="L12" s="6"/>
-      <c r="N12" s="5">
+      <c r="N12" s="6"/>
+      <c r="P12" s="5">
         <v>1000</v>
       </c>
-      <c r="O12">
+      <c r="Q12">
         <v>10</v>
       </c>
-      <c r="P12" s="4">
+      <c r="R12" s="4">
         <v>7.5</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -886,15 +911,15 @@
       <c r="G13" s="1">
         <v>35</v>
       </c>
-      <c r="L13" s="6"/>
-      <c r="N13" s="5" t="s">
+      <c r="N13" s="6"/>
+      <c r="P13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="S13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -913,15 +938,15 @@
       <c r="G14" s="1">
         <v>35</v>
       </c>
-      <c r="L14" s="6"/>
-      <c r="N14" s="5" t="s">
+      <c r="N14" s="6"/>
+      <c r="P14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="S14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -940,26 +965,26 @@
       <c r="G15" s="1">
         <v>35</v>
       </c>
-      <c r="L15" s="6">
+      <c r="N15" s="6">
         <v>42005</v>
       </c>
-      <c r="M15" t="s">
+      <c r="O15" t="s">
         <v>39</v>
       </c>
-      <c r="N15" s="5">
+      <c r="P15" s="5">
         <v>670</v>
       </c>
-      <c r="O15">
+      <c r="Q15">
         <v>80</v>
       </c>
-      <c r="P15" s="4">
+      <c r="R15" s="4">
         <v>1.37</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="S15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -975,43 +1000,43 @@
       <c r="E16" s="2">
         <v>93</v>
       </c>
-      <c r="L16" s="6">
+      <c r="N16" s="6">
         <v>42614</v>
       </c>
-      <c r="M16" s="7">
+      <c r="O16" s="7">
         <v>42887</v>
       </c>
-      <c r="N16" s="5">
+      <c r="P16" s="5">
         <v>2600</v>
       </c>
-      <c r="O16">
+      <c r="Q16">
         <v>52</v>
       </c>
-      <c r="P16" s="4">
+      <c r="R16" s="4">
         <v>1.74</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>44</v>
       </c>
-      <c r="L17" s="6">
+      <c r="N17" s="6">
         <v>41518</v>
       </c>
-      <c r="M17" s="7">
+      <c r="O17" s="7">
         <v>42156</v>
       </c>
-      <c r="N17" s="5">
+      <c r="P17" s="5">
         <v>-1000</v>
       </c>
-      <c r="O17">
+      <c r="Q17">
         <v>63</v>
       </c>
-      <c r="P17" s="4">
+      <c r="R17" s="4">
         <v>0.76</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -1030,43 +1055,43 @@
       <c r="G18" s="1">
         <v>35</v>
       </c>
-      <c r="L18" s="6">
+      <c r="N18" s="6">
         <v>42614</v>
       </c>
-      <c r="M18" s="7">
+      <c r="O18" s="7">
         <v>42887</v>
       </c>
-      <c r="N18" s="5">
+      <c r="P18" s="5">
         <v>1200</v>
       </c>
-      <c r="O18">
+      <c r="Q18">
         <v>27</v>
       </c>
-      <c r="P18" s="4">
+      <c r="R18" s="4">
         <v>1.7</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>44</v>
       </c>
-      <c r="L19" s="6">
+      <c r="N19" s="6">
         <v>41518</v>
       </c>
-      <c r="M19" s="7">
+      <c r="O19" s="7">
         <v>42156</v>
       </c>
-      <c r="N19" s="5">
+      <c r="P19" s="5">
         <v>700</v>
       </c>
-      <c r="O19">
+      <c r="Q19">
         <v>31</v>
       </c>
-      <c r="P19" s="4">
+      <c r="R19" s="4">
         <v>1.5</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -1088,26 +1113,26 @@
       <c r="J20" s="3">
         <v>6000</v>
       </c>
-      <c r="L20" s="6">
+      <c r="N20" s="6">
         <v>42005</v>
       </c>
-      <c r="M20" s="6">
+      <c r="O20" s="6">
         <v>42736</v>
       </c>
-      <c r="N20" s="5">
+      <c r="P20" s="5">
         <v>650</v>
       </c>
-      <c r="O20">
+      <c r="Q20">
         <v>24</v>
       </c>
-      <c r="P20" s="4">
+      <c r="R20" s="4">
         <v>1.44</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="S20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -1129,26 +1154,26 @@
       <c r="J21" s="3">
         <v>6000</v>
       </c>
-      <c r="L21" s="6">
+      <c r="N21" s="6">
         <v>41640</v>
       </c>
-      <c r="M21" s="6">
+      <c r="O21" s="6">
         <v>42370</v>
       </c>
-      <c r="N21" s="5">
+      <c r="P21" s="5">
         <v>670</v>
       </c>
-      <c r="O21">
+      <c r="Q21">
         <v>12</v>
       </c>
-      <c r="P21" s="4">
+      <c r="R21" s="4">
         <v>3</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="S21" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -1170,24 +1195,323 @@
       <c r="J22" s="3">
         <v>6000</v>
       </c>
-      <c r="L22" s="6">
+      <c r="N22" s="6">
         <v>41275</v>
       </c>
-      <c r="M22" s="6">
+      <c r="O22" s="6">
         <v>42005</v>
       </c>
-      <c r="N22" s="5">
+      <c r="P22" s="5">
         <v>1400</v>
       </c>
-      <c r="O22">
+      <c r="Q22">
         <v>128</v>
       </c>
-      <c r="P22" s="4">
+      <c r="R22" s="4">
         <v>1.24</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="S22" t="s">
         <v>48</v>
       </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="2">
+        <v>10</v>
+      </c>
+      <c r="E25" s="2">
+        <v>86</v>
+      </c>
+      <c r="G25" s="1">
+        <v>40</v>
+      </c>
+      <c r="H25" s="3">
+        <v>30</v>
+      </c>
+      <c r="J25" s="3">
+        <v>6000</v>
+      </c>
+      <c r="K25" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="L25" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="N25" s="6">
+        <v>42005</v>
+      </c>
+      <c r="O25" s="6">
+        <v>42370</v>
+      </c>
+      <c r="P25" s="5">
+        <v>640</v>
+      </c>
+      <c r="Q25">
+        <v>28</v>
+      </c>
+      <c r="R25" s="4">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="J26" s="3">
+        <v>8000</v>
+      </c>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="5">
+        <v>590</v>
+      </c>
+      <c r="Q26">
+        <v>20</v>
+      </c>
+      <c r="R26" s="4">
+        <v>2.0499999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>53</v>
+      </c>
+      <c r="J27" s="3">
+        <v>10000</v>
+      </c>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="5">
+        <v>156</v>
+      </c>
+      <c r="Q27">
+        <v>17</v>
+      </c>
+      <c r="R27" s="4">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J28" s="3">
+        <v>14000</v>
+      </c>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="5">
+        <v>243</v>
+      </c>
+      <c r="Q28">
+        <v>17</v>
+      </c>
+      <c r="R28" s="4">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J29" s="3">
+        <v>18000</v>
+      </c>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="5">
+        <v>286</v>
+      </c>
+      <c r="Q29">
+        <v>17</v>
+      </c>
+      <c r="R29" s="4">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J30" s="3">
+        <v>31000</v>
+      </c>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="5">
+        <v>-380</v>
+      </c>
+      <c r="Q30">
+        <v>23</v>
+      </c>
+      <c r="R30" s="4">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="2">
+        <v>10</v>
+      </c>
+      <c r="E33" s="2">
+        <v>92</v>
+      </c>
+      <c r="G33" s="1">
+        <v>35</v>
+      </c>
+      <c r="H33" s="3">
+        <v>20</v>
+      </c>
+      <c r="J33" s="3">
+        <v>18000</v>
+      </c>
+      <c r="K33" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="L33" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="N33" s="6"/>
+      <c r="O33" s="6"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N37" s="6"/>
+      <c r="O37" s="6"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N38" s="6"/>
+      <c r="O38" s="6"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N39" s="6"/>
+      <c r="O39" s="6"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N40" s="6"/>
+      <c r="O40" s="6"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N41" s="6"/>
+      <c r="O41" s="6"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N42" s="6"/>
+      <c r="O42" s="6"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N43" s="6"/>
+      <c r="O43" s="6"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N44" s="6"/>
+      <c r="O44" s="6"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N45" s="6"/>
+      <c r="O45" s="6"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N46" s="6"/>
+      <c r="O46" s="6"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N47" s="6"/>
+      <c r="O47" s="6"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N48" s="6"/>
+      <c r="O48" s="6"/>
+    </row>
+    <row r="49" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N49" s="6"/>
+      <c r="O49" s="6"/>
+    </row>
+    <row r="50" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N50" s="6"/>
+      <c r="O50" s="6"/>
+    </row>
+    <row r="51" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N51" s="6"/>
+      <c r="O51" s="6"/>
+    </row>
+    <row r="52" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N52" s="6"/>
+      <c r="O52" s="6"/>
+    </row>
+    <row r="53" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N53" s="6"/>
+      <c r="O53" s="6"/>
+    </row>
+    <row r="54" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N54" s="6"/>
+      <c r="O54" s="6"/>
+    </row>
+    <row r="55" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N55" s="6"/>
+      <c r="O55" s="6"/>
+    </row>
+    <row r="56" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N56" s="6"/>
+      <c r="O56" s="6"/>
+    </row>
+    <row r="57" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N57" s="6"/>
+      <c r="O57" s="6"/>
+    </row>
+    <row r="58" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N58" s="6"/>
+      <c r="O58" s="6"/>
+    </row>
+    <row r="59" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N59" s="6"/>
+      <c r="O59" s="6"/>
+    </row>
+    <row r="60" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N60" s="6"/>
+      <c r="O60" s="6"/>
+    </row>
+    <row r="61" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N61" s="6"/>
+      <c r="O61" s="6"/>
+    </row>
+    <row r="62" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N62" s="6"/>
+      <c r="O62" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>